<commit_message>
EM-6018 fix search fields
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/CCD_HRS_v1.3-AAT.xlsx
+++ b/src/functionalTest/resources/CCD_HRS_v1.3-AAT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mustafadayican/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mustafadayican/hmcts/em/em-hrs-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1418FE-7781-FF4D-8F4F-995C2160217A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5693A545-45AB-1941-940D-76BE48537F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20420" tabRatio="500" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="334">
   <si>
     <t>Change History</t>
   </si>
@@ -2395,7 +2395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -3311,8 +3311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AMJ21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="143" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="143" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3547,24 +3547,14 @@
       <c r="J9" s="54"/>
     </row>
     <row r="10" spans="1:10" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="23">
-        <v>44197</v>
-      </c>
+      <c r="A10" s="23"/>
       <c r="B10" s="54"/>
-      <c r="C10" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="46" t="s">
-        <v>79</v>
-      </c>
+      <c r="C10" s="39"/>
+      <c r="D10" s="46"/>
       <c r="E10" s="54"/>
-      <c r="F10" s="145" t="s">
-        <v>80</v>
-      </c>
+      <c r="F10" s="145"/>
       <c r="G10" s="54"/>
-      <c r="H10" s="62">
-        <v>8</v>
-      </c>
+      <c r="H10" s="62"/>
       <c r="I10" s="54"/>
       <c r="J10" s="54"/>
     </row>
@@ -3995,7 +3985,7 @@
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -4251,24 +4241,14 @@
       <c r="J10" s="54"/>
     </row>
     <row r="11" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="23">
-        <v>44197</v>
-      </c>
+      <c r="A11" s="23"/>
       <c r="B11" s="24"/>
-      <c r="C11" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="46" t="s">
-        <v>79</v>
-      </c>
+      <c r="C11" s="39"/>
+      <c r="D11" s="46"/>
       <c r="E11" s="24"/>
-      <c r="F11" s="46" t="s">
-        <v>80</v>
-      </c>
+      <c r="F11" s="46"/>
       <c r="G11" s="24"/>
-      <c r="H11" s="62">
-        <v>9</v>
-      </c>
+      <c r="H11" s="62"/>
       <c r="I11" s="116"/>
       <c r="J11" s="54"/>
     </row>
@@ -4285,7 +4265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AMJ14"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="H2" zoomScale="161" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="161" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>